<commit_message>
Have various validation results saved. Could pick parameters from one of those as the final model to test on.
</commit_message>
<xml_diff>
--- a/src/pytorch/results/New Dataset/Results.xlsx
+++ b/src/pytorch/results/New Dataset/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luc\Documents\CPS 803\Main Project\src\pytorch\results\New Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AADF559-DB5C-4C5D-A3F1-D1EC59D02BA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39AFE494-514C-4DF5-A687-DAC83F605BF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
   <si>
     <t>Batch Size</t>
   </si>
@@ -38,6 +38,207 @@
   </si>
   <si>
     <t>Accuracy of Enemy</t>
+  </si>
+  <si>
+    <t>[85.01]</t>
+  </si>
+  <si>
+    <t>[88.3]</t>
+  </si>
+  <si>
+    <t>[82.2]</t>
+  </si>
+  <si>
+    <t>[83.97]</t>
+  </si>
+  <si>
+    <t>[82.84]</t>
+  </si>
+  <si>
+    <t>[84.85]</t>
+  </si>
+  <si>
+    <t>[85.87]</t>
+  </si>
+  <si>
+    <t>[85.6]</t>
+  </si>
+  <si>
+    <t>[85.73]</t>
+  </si>
+  <si>
+    <t>[85.48]</t>
+  </si>
+  <si>
+    <t>[78.35]</t>
+  </si>
+  <si>
+    <t>[91.25]</t>
+  </si>
+  <si>
+    <t>[83.33]</t>
+  </si>
+  <si>
+    <t>[78.02]</t>
+  </si>
+  <si>
+    <t>[86.3]</t>
+  </si>
+  <si>
+    <t>[84.17]</t>
+  </si>
+  <si>
+    <t>[79.78]</t>
+  </si>
+  <si>
+    <t>[88.42]</t>
+  </si>
+  <si>
+    <t>[83.28]</t>
+  </si>
+  <si>
+    <t>[83.49]</t>
+  </si>
+  <si>
+    <t>[82.67]</t>
+  </si>
+  <si>
+    <t>[77.38]</t>
+  </si>
+  <si>
+    <t>[85.68]</t>
+  </si>
+  <si>
+    <t>[71.88]</t>
+  </si>
+  <si>
+    <t>[77.1]</t>
+  </si>
+  <si>
+    <t>[72.14]</t>
+  </si>
+  <si>
+    <t>[81.44]</t>
+  </si>
+  <si>
+    <t>[79.25]</t>
+  </si>
+  <si>
+    <t>[75.92]</t>
+  </si>
+  <si>
+    <t>[83.4]</t>
+  </si>
+  <si>
+    <t>[72.93]</t>
+  </si>
+  <si>
+    <t>[92.8]</t>
+  </si>
+  <si>
+    <t>[82.28]</t>
+  </si>
+  <si>
+    <t>[77.12]</t>
+  </si>
+  <si>
+    <t>[86.27]</t>
+  </si>
+  <si>
+    <t>[84.51]</t>
+  </si>
+  <si>
+    <t>[77.52]</t>
+  </si>
+  <si>
+    <t>[90.25]</t>
+  </si>
+  <si>
+    <t>[80.3]</t>
+  </si>
+  <si>
+    <t>[70.65]</t>
+  </si>
+  <si>
+    <t>[87.92]</t>
+  </si>
+  <si>
+    <t>[80.05]</t>
+  </si>
+  <si>
+    <t>[86.18]</t>
+  </si>
+  <si>
+    <t>[76.1]</t>
+  </si>
+  <si>
+    <t>[79.76]</t>
+  </si>
+  <si>
+    <t>[82.07]</t>
+  </si>
+  <si>
+    <t>[77.59]</t>
+  </si>
+  <si>
+    <t>[86.33]</t>
+  </si>
+  <si>
+    <t>[87.9]</t>
+  </si>
+  <si>
+    <t>[84.89]</t>
+  </si>
+  <si>
+    <t>[87.23]</t>
+  </si>
+  <si>
+    <t>[83.04]</t>
+  </si>
+  <si>
+    <t>[90.81]</t>
+  </si>
+  <si>
+    <t>[80.59]</t>
+  </si>
+  <si>
+    <t>[88.92]</t>
+  </si>
+  <si>
+    <t>[73.77]</t>
+  </si>
+  <si>
+    <t>[84.66]</t>
+  </si>
+  <si>
+    <t>[73.03]</t>
+  </si>
+  <si>
+    <t>[94.07]</t>
+  </si>
+  <si>
+    <t>[85.23]</t>
+  </si>
+  <si>
+    <t>[75.45]</t>
+  </si>
+  <si>
+    <t>[94.31]</t>
+  </si>
+  <si>
+    <t>[82.26]</t>
+  </si>
+  <si>
+    <t>[68.31]</t>
+  </si>
+  <si>
+    <t>[93.99]</t>
+  </si>
+  <si>
+    <t>[87.59]</t>
+  </si>
+  <si>
+    <t>[79.01]</t>
   </si>
 </sst>
 </file>
@@ -400,20 +601,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -436,6 +635,466 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1E-3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1E-3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1E-3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1E-3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1E-3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1E-3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1E-3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>32</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1E-3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>64</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1E-3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" t="s">
+        <v>69</v>
+      </c>
+      <c r="F25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" t="s">
+        <v>71</v>
+      </c>
+      <c r="F26" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Final results have been recorded.
</commit_message>
<xml_diff>
--- a/src/pytorch/results/New Dataset/Results.xlsx
+++ b/src/pytorch/results/New Dataset/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luc\Documents\CPS 803\Main Project\src\pytorch\results\New Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39AFE494-514C-4DF5-A687-DAC83F605BF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CC4DBF-2943-4BF9-884A-62B96050D573}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
   <si>
     <t>Batch Size</t>
   </si>
@@ -239,13 +239,19 @@
   </si>
   <si>
     <t>[79.01]</t>
+  </si>
+  <si>
+    <t>Final Testing of Model</t>
+  </si>
+  <si>
+    <t>Validation of Models</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,6 +263,14 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -294,10 +308,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -601,83 +622,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1E-3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1E-3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -686,18 +678,18 @@
         <v>1E-3</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -706,18 +698,18 @@
         <v>1E-3</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -726,18 +718,18 @@
         <v>1E-3</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -746,18 +738,18 @@
         <v>1E-3</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -766,18 +758,18 @@
         <v>1E-3</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -786,18 +778,18 @@
         <v>1E-3</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -806,58 +798,58 @@
         <v>1E-3</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>32</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1E-3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12">
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>5</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -866,18 +858,18 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="F14" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -886,18 +878,18 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F15" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -906,18 +898,18 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F16" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -926,18 +918,18 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F17" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -946,58 +938,58 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="D18" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E18" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F18" t="s">
-        <v>52</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20">
-        <v>8.9999999999999993E-3</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F20" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>5</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="D21" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21" t="s">
-        <v>57</v>
-      </c>
-      <c r="F21" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -1006,38 +998,38 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="D22" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E22" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F22" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>7</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23">
+      <c r="A23" s="2">
+        <v>5</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="D23" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" t="s">
-        <v>63</v>
-      </c>
-      <c r="F23" t="s">
-        <v>64</v>
+      <c r="D23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1046,18 +1038,18 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E24" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F24" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1066,18 +1058,18 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="D25" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E25" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F25" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -1086,16 +1078,111 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="D26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>9</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>10</v>
       </c>
-      <c r="E26" t="s">
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" t="s">
         <v>71</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F28" t="s">
         <v>72</v>
       </c>
     </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>5</v>
+      </c>
+      <c r="B32" s="4">
+        <v>1</v>
+      </c>
+      <c r="C32" s="4">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="D32" s="4">
+        <v>86.69</v>
+      </c>
+      <c r="E32" s="4">
+        <v>84.7</v>
+      </c>
+      <c r="F32" s="4">
+        <v>88.61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>5</v>
+      </c>
+      <c r="B33" s="4">
+        <v>5</v>
+      </c>
+      <c r="C33" s="4">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="D33" s="4">
+        <v>98.73</v>
+      </c>
+      <c r="E33" s="4">
+        <v>98.1</v>
+      </c>
+      <c r="F33" s="4">
+        <v>99.27</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a line of clarification to the results spreadsheet
</commit_message>
<xml_diff>
--- a/src/pytorch/results/New Dataset/Results.xlsx
+++ b/src/pytorch/results/New Dataset/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luc\Documents\CPS 803\Main Project\src\pytorch\results\New Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CC4DBF-2943-4BF9-884A-62B96050D573}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787CA25D-7096-4A9D-85FC-00B6F3E27733}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
   <si>
     <t>Batch Size</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t>Validation of Models</t>
+  </si>
+  <si>
+    <t>Chosen model to test on</t>
   </si>
 </sst>
 </file>
@@ -314,10 +317,10 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -622,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,14 +641,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -907,7 +910,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>7</v>
       </c>
@@ -927,7 +930,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>8</v>
       </c>
@@ -947,7 +950,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>9</v>
       </c>
@@ -967,7 +970,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>10</v>
       </c>
@@ -987,7 +990,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4</v>
       </c>
@@ -1007,7 +1010,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>5</v>
       </c>
@@ -1026,8 +1029,11 @@
       <c r="F23" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6</v>
       </c>
@@ -1047,7 +1053,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>7</v>
       </c>
@@ -1067,7 +1073,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>8</v>
       </c>
@@ -1087,7 +1093,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>9</v>
       </c>
@@ -1107,7 +1113,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>10</v>
       </c>
@@ -1127,53 +1133,53 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
         <v>5</v>
       </c>
-      <c r="B32" s="4">
-        <v>1</v>
-      </c>
-      <c r="C32" s="4">
+      <c r="B32" s="3">
+        <v>1</v>
+      </c>
+      <c r="C32" s="3">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="3">
         <v>86.69</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E32" s="3">
         <v>84.7</v>
       </c>
-      <c r="F32" s="4">
+      <c r="F32" s="3">
         <v>88.61</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+      <c r="A33" s="3">
         <v>5</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="3">
         <v>5</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="3">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="3">
         <v>98.73</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="3">
         <v>98.1</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F33" s="3">
         <v>99.27</v>
       </c>
     </row>

</xml_diff>